<commit_message>
feat: Conclusion of report and notebook
</commit_message>
<xml_diff>
--- a/resultados/ComparaçãoModelos.xlsx
+++ b/resultados/ComparaçãoModelos.xlsx
@@ -453,105 +453,105 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ridge</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.7198802954187024</v>
+        <v>-0.6964138191236289</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07584433058155739</v>
+        <v>0.1214519707733044</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Regressão Linear</t>
+          <t>AdaBoost</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.7508734574409605</v>
+        <v>-0.7130459633531724</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08872533313648187</v>
+        <v>0.1126153033697651</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>Gradient Boosting</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.7672494840868467</v>
+        <v>-0.7428176167041384</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1567336281309491</v>
+        <v>0.1228843929285316</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gradient Boosting</t>
+          <t>Ridge</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.817628067242657</v>
+        <v>-0.7582896788257542</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09834777485372839</v>
+        <v>0.08934969879638968</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AdaBoost</t>
+          <t>Regressão Linear</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.820469343033514</v>
+        <v>-0.786326437207539</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1604323807442088</v>
+        <v>0.09764696779109285</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lasso</t>
+          <t>Árvore de Decisão</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.9573421825625668</v>
+        <v>-0.9028735991172265</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2293965961906358</v>
+        <v>0.2532394192359003</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Lasso</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.9798617634341792</v>
+        <v>-1.000047922155725</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2297864448895982</v>
+        <v>0.2289771620612693</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Árvore de Decisão</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.9913625642415841</v>
+        <v>-1.024527499566607</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2261635968334492</v>
+        <v>0.2297887073710829</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-27.12709805760273</v>
+        <v>-64.89742225138278</v>
       </c>
       <c r="C10" t="n">
-        <v>32.01605714078701</v>
+        <v>10.82065414368644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>